<commit_message>
generate triple cuts only for top 20% areas with most population
</commit_message>
<xml_diff>
--- a/Results/2023-12-13_23-56-21_Joplin_150Clusters_Budget15M_5.0Miles.xlsx
+++ b/Results/2023-12-13_23-56-21_Joplin_150Clusters_Budget15M_5.0Miles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54082C0C-F467-490D-BBB8-00E0234F1A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5A94EC-49D2-4A82-B93D-8421D894EA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-12-13_23-56-21_Joplin_150C" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -651,23 +651,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>609143</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>152105</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{233516D9-B0E6-39D8-7990-DA160860CAA2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6F43905-453D-02D0-F119-F12978A568C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -683,7 +683,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4267200" y="184150"/>
+          <a:off x="6096000" y="0"/>
           <a:ext cx="3657143" cy="2361905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -992,11 +992,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1020,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12143</v>
+        <v>12167</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1028,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>12666</v>
+        <v>12256</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1036,7 +1036,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1044,7 +1044,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>4921.13</v>
+        <v>2272.23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1052,7 +1052,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1060,7 +1060,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>4920.58</v>
+        <v>2270.83</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1068,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>78</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1076,7 +1076,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>20.27</v>
+        <v>18.48</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1092,7 +1092,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>9.2899999999999991</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1218,10 +1218,10 @@
         <v>393</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>119127</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
@@ -1392,10 +1392,10 @@
         <v>379</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F24">
-        <v>98122</v>
+        <v>176124</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
@@ -1421,10 +1421,10 @@
         <v>251</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>74746</v>
       </c>
       <c r="G25" t="s">
         <v>24</v>
@@ -1807,10 +1807,10 @@
         <v>26</v>
       </c>
       <c r="H38">
-        <v>2674315</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>187</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -2204,10 +2204,10 @@
         <v>480</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>83825</v>
       </c>
       <c r="G52" t="s">
         <v>24</v>
@@ -2233,10 +2233,10 @@
         <v>510</v>
       </c>
       <c r="E53" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>84491</v>
       </c>
       <c r="G53" t="s">
         <v>24</v>
@@ -2320,10 +2320,10 @@
         <v>336</v>
       </c>
       <c r="E56" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>70403</v>
       </c>
       <c r="G56" t="s">
         <v>24</v>
@@ -2523,10 +2523,10 @@
         <v>463</v>
       </c>
       <c r="E63" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>69969</v>
       </c>
       <c r="G63" t="s">
         <v>24</v>
@@ -2610,10 +2610,10 @@
         <v>698</v>
       </c>
       <c r="E66" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>134681</v>
       </c>
       <c r="G66" t="s">
         <v>24</v>
@@ -2668,10 +2668,10 @@
         <v>605</v>
       </c>
       <c r="E68" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>95898</v>
       </c>
       <c r="G68" t="s">
         <v>24</v>
@@ -2697,10 +2697,10 @@
         <v>507</v>
       </c>
       <c r="E69" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>95286</v>
       </c>
       <c r="G69" t="s">
         <v>24</v>
@@ -2842,10 +2842,10 @@
         <v>315</v>
       </c>
       <c r="E74" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>72782</v>
       </c>
       <c r="G74" t="s">
         <v>24</v>
@@ -2871,10 +2871,10 @@
         <v>264</v>
       </c>
       <c r="E75" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>49089</v>
       </c>
       <c r="G75" t="s">
         <v>24</v>
@@ -3480,10 +3480,10 @@
         <v>230</v>
       </c>
       <c r="E96" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F96">
-        <v>95064</v>
+        <v>52961</v>
       </c>
       <c r="G96" t="s">
         <v>26</v>
@@ -3492,7 +3492,7 @@
         <v>0</v>
       </c>
       <c r="I96">
-        <v>187</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -4620,10 +4620,10 @@
         <v>26</v>
       </c>
       <c r="H135">
-        <v>0</v>
+        <v>2211052</v>
       </c>
       <c r="I135">
-        <v>199</v>
+        <v>154</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
@@ -4727,10 +4727,10 @@
         <v>778</v>
       </c>
       <c r="E139" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F139">
-        <v>317336</v>
+        <v>176794</v>
       </c>
       <c r="G139" t="s">
         <v>24</v>
@@ -4843,10 +4843,10 @@
         <v>410</v>
       </c>
       <c r="E143" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F143">
-        <v>197631</v>
+        <v>110102</v>
       </c>
       <c r="G143" t="s">
         <v>24</v>
@@ -5075,10 +5075,10 @@
         <v>458</v>
       </c>
       <c r="E151" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F151">
-        <v>0</v>
+        <v>152780</v>
       </c>
       <c r="G151" t="s">
         <v>24</v>

</xml_diff>